<commit_message>
Card data writing is excel is done.
</commit_message>
<xml_diff>
--- a/datafiles/cardData.xlsx
+++ b/datafiles/cardData.xlsx
@@ -2,40 +2,45 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gourav.sharma\IdeaProjects\falcon_project\datafiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
-  <si>
-    <t>CardID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>b2175ce7-ac92-4073-bfd7-6eb30f992353</t>
   </si>
+  <si>
+    <t>e6c063f2-9c99-4f42-ad74-574fbacd06a3</t>
+  </si>
+  <si>
+    <t>c2107520-2f9f-4ce4-b67d-211e61b3357c</t>
+  </si>
+  <si>
+    <t>868b681d-92b0-4c69-931d-6b0a0dcbce2c</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -343,29 +348,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A2:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>